<commit_message>
Update with token state in DB Open-source the generator codes!
</commit_message>
<xml_diff>
--- a/doc/database.xlsx
+++ b/doc/database.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Deviser\dev-doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93BD59B-E32C-4B54-9016-759F5D4111C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A49175-9655-41CA-9A64-AF1E86953D5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="150" windowWidth="13800" windowHeight="15225" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="435" yWindow="945" windowWidth="13800" windowHeight="14220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
-    <sheet name="acl" sheetId="5" r:id="rId2"/>
-    <sheet name="account" sheetId="3" r:id="rId3"/>
-    <sheet name="audit" sheetId="4" r:id="rId4"/>
-    <sheet name="test" sheetId="6" r:id="rId5"/>
+    <sheet name="account" sheetId="3" r:id="rId2"/>
+    <sheet name="token" sheetId="7" r:id="rId3"/>
+    <sheet name="acl" sheetId="5" r:id="rId4"/>
+    <sheet name="audit" sheetId="4" r:id="rId5"/>
+    <sheet name="test" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="56">
   <si>
     <t>Database Name</t>
   </si>
@@ -191,6 +192,12 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>uuid</t>
+  </si>
+  <si>
+    <t>token</t>
   </si>
 </sst>
 </file>
@@ -552,7 +559,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,11 +686,315 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBC2075-6ABD-479F-B898-3062C6C311BD}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="6">
+        <v>32</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="6">
+        <v>128</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6">
+        <v>32</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="6">
+        <v>16</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E5:H8" xr:uid="{55145CA6-35EE-4105-A6E5-F32B02B7FAA1}">
+      <formula1>"No,Yes"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B8" xr:uid="{13AD8084-39D1-497C-8AC4-D548B197CF67}">
+      <formula1>"VARCHAR,INT,DECIMAL,BLOB,BOOLEAN,DATETIME,AUTO"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7A958FE-BC38-4B17-9FA6-5F45D5061A58}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="6">
+        <v>64</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="6">
+        <v>32</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6">
+        <v>16</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B7" xr:uid="{31497EE6-5949-4235-958D-8C33E189B068}">
+      <formula1>"VARCHAR,INT,DECIMAL,BLOB,BOOLEAN,DATETIME,AUTO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E5:H7" xr:uid="{58059BA5-CEA2-4F78-9FF6-F44D3331EE2C}">
+      <formula1>"No,Yes"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAEDFA54-A04E-40B1-A006-206FB25BB047}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,172 +1132,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBC2075-6ABD-479F-B898-3062C6C311BD}">
-  <dimension ref="A1:H8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="6">
-        <v>32</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="6">
-        <v>16</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="6">
-        <v>32</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="6">
-        <v>16</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E5:H8" xr:uid="{55145CA6-35EE-4105-A6E5-F32B02B7FAA1}">
-      <formula1>"No,Yes"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B8" xr:uid="{13AD8084-39D1-497C-8AC4-D548B197CF67}">
-      <formula1>"VARCHAR,INT,DECIMAL,BLOB,BOOLEAN,DATETIME,AUTO"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CEE687E-5DD2-48B8-ABB4-DFB6D3FE6769}">
   <dimension ref="A1:H8"/>
   <sheetViews>
@@ -1149,11 +1295,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{680252D9-1E5E-453E-AAF3-388A4214432A}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>

</xml_diff>